<commit_message>
jacobian error fixed, rotation correct
</commit_message>
<xml_diff>
--- a/conven_control/data/non_optimized_curved.xlsx
+++ b/conven_control/data/non_optimized_curved.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>J1</t>
   </si>
@@ -46,10 +46,7 @@
     <t>dz</t>
   </si>
   <si>
-    <t>[ 0.7238 -0.0505 -0.2786 -0.0023 -0.9307  0.0024 -0.3658]</t>
-  </si>
-  <si>
-    <t>[ 0.7238 -0.0505 -0.2786  0.0024  0.9307 -0.0025  0.3659]</t>
+    <t>[   0.7238   -0.0505   -0.278  -122.4354   42.8765  179.7921]</t>
   </si>
 </sst>
 </file>
@@ -407,7 +404,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -450,69 +447,34 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>-7.861</v>
+        <v>4.938</v>
       </c>
       <c r="C2">
-        <v>52.651</v>
+        <v>66.63</v>
       </c>
       <c r="D2">
-        <v>74.70399999999999</v>
+        <v>59.243</v>
       </c>
       <c r="E2">
-        <v>-153.235</v>
+        <v>-80.26900000000001</v>
       </c>
       <c r="F2">
-        <v>-11.125</v>
+        <v>62.379</v>
       </c>
       <c r="G2">
-        <v>148.052</v>
+        <v>77.441</v>
       </c>
       <c r="H2" t="s">
         <v>10</v>
       </c>
       <c r="I2">
-        <v>3.482</v>
+        <v>3.369</v>
       </c>
       <c r="J2">
-        <v>-0.575</v>
+        <v>0.054</v>
       </c>
       <c r="K2">
-        <v>7.548</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>-7.858</v>
-      </c>
-      <c r="C3">
-        <v>52.649</v>
-      </c>
-      <c r="D3">
-        <v>74.709</v>
-      </c>
-      <c r="E3">
-        <v>-153.283</v>
-      </c>
-      <c r="F3">
-        <v>-11.112</v>
-      </c>
-      <c r="G3">
-        <v>148.105</v>
-      </c>
-      <c r="H3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3">
-        <v>3.482</v>
-      </c>
-      <c r="J3">
-        <v>-0.575</v>
-      </c>
-      <c r="K3">
-        <v>7.548</v>
+        <v>7.825</v>
       </c>
     </row>
   </sheetData>

</xml_diff>